<commit_message>
Versão final do Bot de Alertas com Google Sheets
</commit_message>
<xml_diff>
--- a/Base_tecnicos.xlsx
+++ b/Base_tecnicos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\w.soares\Desktop\bot-alertas-whatsapp\bot-alertas-whatsapp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\w.soares\Desktop\bot_alertas_whatsapp_FINAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA50390-FB93-4423-9D1D-51AE84F2AF77}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2C1910-D07C-4B32-B593-2FA77C9377D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15200" windowHeight="6810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2011,8 +2011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C130" sqref="B130:C130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5678,7 +5678,7 @@
         <v>11</v>
       </c>
       <c r="C130" s="2">
-        <v>21974508325</v>
+        <v>21974197468</v>
       </c>
       <c r="D130" t="s">
         <v>12</v>

</xml_diff>